<commit_message>
[main] continued to work on report
Branch: [main]
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BA computer science\year 3\semB\intro to ai\AI_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BA Computer Science\Year 3\Sem B\intro to ai\AI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384E5E94-B76C-4803-B16C-5DF125D41444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193FD6A8-6CEB-47D2-B8C6-80F4CCF69121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{825CD43D-022B-4D40-A0AD-AF1AEE1DDB0E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{825CD43D-022B-4D40-A0AD-AF1AEE1DDB0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>alpha_beta vs offensive</t>
   </si>
@@ -66,6 +66,24 @@
   </si>
   <si>
     <t>rl trained without master</t>
+  </si>
+  <si>
+    <t>complex</t>
+  </si>
+  <si>
+    <t>only_best_opponent</t>
+  </si>
+  <si>
+    <t>vs 2 offensive</t>
+  </si>
+  <si>
+    <t>vs 2 defensive</t>
+  </si>
+  <si>
+    <t>vs offensive, defensive</t>
+  </si>
+  <si>
+    <t>vs offensive, random</t>
   </si>
 </sst>
 </file>
@@ -633,7 +651,516 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Compare heiuristic with 3 players</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>complex</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$11:$R$11</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>vs 2 offensive</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>vs 2 defensive</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>vs offensive, defensive</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>vs offensive, random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$12:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-385F-4F69-A849-2B9657C1B1A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>only_best_opponent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$11:$R$11</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>vs 2 offensive</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>vs 2 defensive</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>vs offensive, defensive</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>vs offensive, random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$13:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-385F-4F69-A849-2B9657C1B1A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1493409199"/>
+        <c:axId val="1493417839"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1493409199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1493417839"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1493417839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>winning percentage (on 100 games)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1493409199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1176,6 +1703,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1209,6 +2239,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1109662</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1004887</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E2334A1-38F1-E275-831A-7CC396D6E6B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1534,29 +2600,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC9DC5B-6E06-4CB7-9EBF-6BF683D352A4}">
-  <dimension ref="A2:M8"/>
+  <dimension ref="A2:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J3" t="s">
         <v>5</v>
       </c>
@@ -1570,7 +2641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1596,7 +2667,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.6</v>
       </c>
@@ -1622,7 +2693,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -1633,7 +2704,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.2</v>
       </c>
@@ -1644,7 +2715,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1653,6 +2724,54 @@
       </c>
       <c r="C8">
         <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>93</v>
+      </c>
+      <c r="P12">
+        <v>84</v>
+      </c>
+      <c r="Q12">
+        <v>82</v>
+      </c>
+      <c r="R12">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13">
+        <v>90</v>
+      </c>
+      <c r="P13">
+        <v>76</v>
+      </c>
+      <c r="Q13">
+        <v>74</v>
+      </c>
+      <c r="R13">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[complex_consider_depths] edited report and charts
Branch: [complex_consider_depths]
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BA Computer Science\Year 3\Sem B\intro to ai\AI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193FD6A8-6CEB-47D2-B8C6-80F4CCF69121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405DA67F-0744-4B55-8AED-31D3EE2D7842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{825CD43D-022B-4D40-A0AD-AF1AEE1DDB0E}"/>
   </bookViews>
@@ -382,36 +382,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -460,6 +430,7 @@
         <c:axId val="1556551967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -937,6 +908,7 @@
         <c:axId val="1493417839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2602,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC9DC5B-6E06-4CB7-9EBF-6BF683D352A4}">
   <dimension ref="A2:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[main] edited report and charts
Branch: [main]
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BA Computer Science\Year 3\Sem B\intro to ai\AI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193FD6A8-6CEB-47D2-B8C6-80F4CCF69121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405DA67F-0744-4B55-8AED-31D3EE2D7842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{825CD43D-022B-4D40-A0AD-AF1AEE1DDB0E}"/>
   </bookViews>
@@ -382,36 +382,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -460,6 +430,7 @@
         <c:axId val="1556551967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -937,6 +908,7 @@
         <c:axId val="1493417839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2602,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC9DC5B-6E06-4CB7-9EBF-6BF683D352A4}">
   <dimension ref="A2:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>